<commit_message>
Porting chapter 2 to python 3 - part 2
</commit_message>
<xml_diff>
--- a/Chapter_2_Code/Data/mtcars_new.xlsx
+++ b/Chapter_2_Code/Data/mtcars_new.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>model</t>
   </si>
@@ -152,26 +153,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -186,35 +183,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -502,12 +490,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
@@ -551,37 +545,37 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>21</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>160</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>110</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>3.9</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>2.62</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>16.46</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="L2">
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4</v>
+      </c>
+      <c r="L2" t="n">
         <v>4</v>
       </c>
     </row>
@@ -589,37 +583,37 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>21</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>160</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>110</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>3.9</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>2.875</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>17.02</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
-      </c>
-      <c r="L3">
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L3" t="n">
         <v>4</v>
       </c>
     </row>
@@ -627,37 +621,37 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>22.8</v>
       </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
         <v>108</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>93</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>3.85</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>2.32</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="n">
         <v>18.61</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
-      </c>
-      <c r="L4">
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -665,37 +659,37 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>21.4</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>6</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>258</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>110</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>3.08</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>3.215</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>19.44</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>3</v>
-      </c>
-      <c r="L5">
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3</v>
+      </c>
+      <c r="L5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -703,37 +697,37 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>18.7</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>8</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>360</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>175</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>3.15</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>3.44</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="n">
         <v>17.02</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>3</v>
-      </c>
-      <c r="L6">
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" t="n">
         <v>2</v>
       </c>
     </row>
@@ -741,37 +735,37 @@
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>18.1</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>6</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>225</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>105</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>2.76</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="n">
         <v>3.46</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="n">
         <v>20.22</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
-      <c r="L7">
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>3</v>
+      </c>
+      <c r="L7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -779,37 +773,37 @@
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>14.3</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>360</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>245</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="n">
         <v>3.21</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="n">
         <v>3.57</v>
       </c>
-      <c r="H8">
+      <c r="H8" t="n">
         <v>15.84</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
-      <c r="L8">
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>3</v>
+      </c>
+      <c r="L8" t="n">
         <v>4</v>
       </c>
     </row>
@@ -817,37 +811,37 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>24.4</v>
       </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
         <v>146.7</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>62</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="n">
         <v>3.69</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n">
         <v>3.19</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="n">
         <v>20</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>4</v>
-      </c>
-      <c r="L9">
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>4</v>
+      </c>
+      <c r="L9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -855,37 +849,37 @@
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>22.8</v>
       </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="n">
         <v>140.8</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>95</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="n">
         <v>3.92</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="n">
         <v>3.15</v>
       </c>
-      <c r="H10">
+      <c r="H10" t="n">
         <v>22.9</v>
       </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>4</v>
-      </c>
-      <c r="L10">
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>4</v>
+      </c>
+      <c r="L10" t="n">
         <v>2</v>
       </c>
     </row>
@@ -893,37 +887,37 @@
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>19.2</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>6</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>167.6</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>123</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="n">
         <v>3.92</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="n">
         <v>3.44</v>
       </c>
-      <c r="H11">
+      <c r="H11" t="n">
         <v>18.3</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>4</v>
-      </c>
-      <c r="L11">
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>4</v>
+      </c>
+      <c r="L11" t="n">
         <v>4</v>
       </c>
     </row>
@@ -931,37 +925,37 @@
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>17.8</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>6</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>167.6</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>123</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="n">
         <v>3.92</v>
       </c>
-      <c r="G12">
+      <c r="G12" t="n">
         <v>3.44</v>
       </c>
-      <c r="H12">
+      <c r="H12" t="n">
         <v>18.9</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>4</v>
-      </c>
-      <c r="L12">
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>4</v>
+      </c>
+      <c r="L12" t="n">
         <v>4</v>
       </c>
     </row>
@@ -969,37 +963,37 @@
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>16.4</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="n">
         <v>8</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="n">
         <v>275.8</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>180</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="n">
         <v>3.07</v>
       </c>
-      <c r="G13">
+      <c r="G13" t="n">
         <v>4.07</v>
       </c>
-      <c r="H13">
+      <c r="H13" t="n">
         <v>17.4</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>3</v>
-      </c>
-      <c r="L13">
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>3</v>
+      </c>
+      <c r="L13" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1007,37 +1001,37 @@
       <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>17.3</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>8</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>275.8</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>180</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="n">
         <v>3.07</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="n">
         <v>3.73</v>
       </c>
-      <c r="H14">
+      <c r="H14" t="n">
         <v>17.6</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>3</v>
-      </c>
-      <c r="L14">
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3</v>
+      </c>
+      <c r="L14" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1045,37 +1039,37 @@
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>15.2</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>8</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="n">
         <v>275.8</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>180</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="n">
         <v>3.07</v>
       </c>
-      <c r="G15">
+      <c r="G15" t="n">
         <v>3.78</v>
       </c>
-      <c r="H15">
+      <c r="H15" t="n">
         <v>18</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>3</v>
-      </c>
-      <c r="L15">
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1083,37 +1077,37 @@
       <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>10.4</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>8</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>472</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>205</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="n">
         <v>2.93</v>
       </c>
-      <c r="G16">
+      <c r="G16" t="n">
         <v>5.25</v>
       </c>
-      <c r="H16">
+      <c r="H16" t="n">
         <v>17.98</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>3</v>
-      </c>
-      <c r="L16">
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>3</v>
+      </c>
+      <c r="L16" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1121,37 +1115,37 @@
       <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>10.4</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="n">
         <v>8</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="n">
         <v>460</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="n">
         <v>215</v>
       </c>
-      <c r="F17">
-        <v>3</v>
-      </c>
-      <c r="G17">
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" t="n">
         <v>5.424</v>
       </c>
-      <c r="H17">
+      <c r="H17" t="n">
         <v>17.82</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>3</v>
-      </c>
-      <c r="L17">
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>3</v>
+      </c>
+      <c r="L17" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1159,37 +1153,37 @@
       <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>14.7</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>8</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="n">
         <v>440</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>230</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="n">
         <v>3.23</v>
       </c>
-      <c r="G18">
+      <c r="G18" t="n">
         <v>5.345</v>
       </c>
-      <c r="H18">
+      <c r="H18" t="n">
         <v>17.42</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>3</v>
-      </c>
-      <c r="L18">
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>3</v>
+      </c>
+      <c r="L18" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1197,37 +1191,37 @@
       <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="n">
         <v>32.4</v>
       </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
+      <c r="C19" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" t="n">
         <v>78.7</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>66</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="n">
         <v>4.08</v>
       </c>
-      <c r="G19">
+      <c r="G19" t="n">
         <v>2.2</v>
       </c>
-      <c r="H19">
+      <c r="H19" t="n">
         <v>19.47</v>
       </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>4</v>
-      </c>
-      <c r="L19">
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>4</v>
+      </c>
+      <c r="L19" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1235,37 +1229,37 @@
       <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>30.4</v>
       </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20">
+      <c r="C20" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="n">
         <v>75.7</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="n">
         <v>52</v>
       </c>
-      <c r="F20">
+      <c r="F20" t="n">
         <v>4.93</v>
       </c>
-      <c r="G20">
+      <c r="G20" t="n">
         <v>1.615</v>
       </c>
-      <c r="H20">
+      <c r="H20" t="n">
         <v>18.52</v>
       </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>4</v>
-      </c>
-      <c r="L20">
+      <c r="I20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" t="n">
+        <v>4</v>
+      </c>
+      <c r="L20" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1273,37 +1267,37 @@
       <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>33.9</v>
       </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21">
-        <v>71.1</v>
-      </c>
-      <c r="E21">
+      <c r="C21" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" t="n">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="E21" t="n">
         <v>65</v>
       </c>
-      <c r="F21">
+      <c r="F21" t="n">
         <v>4.22</v>
       </c>
-      <c r="G21">
+      <c r="G21" t="n">
         <v>1.835</v>
       </c>
-      <c r="H21">
+      <c r="H21" t="n">
         <v>19.9</v>
       </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>4</v>
-      </c>
-      <c r="L21">
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>4</v>
+      </c>
+      <c r="L21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1311,37 +1305,37 @@
       <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>21.5</v>
       </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22">
+      <c r="C22" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" t="n">
         <v>120.1</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="n">
         <v>97</v>
       </c>
-      <c r="F22">
+      <c r="F22" t="n">
         <v>3.7</v>
       </c>
-      <c r="G22">
+      <c r="G22" t="n">
         <v>2.465</v>
       </c>
-      <c r="H22">
+      <c r="H22" t="n">
         <v>20.01</v>
       </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>3</v>
-      </c>
-      <c r="L22">
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>3</v>
+      </c>
+      <c r="L22" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1349,37 +1343,37 @@
       <c r="A23" t="s">
         <v>33</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="n">
         <v>15.5</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="n">
         <v>8</v>
       </c>
-      <c r="D23">
+      <c r="D23" t="n">
         <v>318</v>
       </c>
-      <c r="E23">
+      <c r="E23" t="n">
         <v>150</v>
       </c>
-      <c r="F23">
+      <c r="F23" t="n">
         <v>2.76</v>
       </c>
-      <c r="G23">
+      <c r="G23" t="n">
         <v>3.52</v>
       </c>
-      <c r="H23">
+      <c r="H23" t="n">
         <v>16.87</v>
       </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>3</v>
-      </c>
-      <c r="L23">
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>3</v>
+      </c>
+      <c r="L23" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1387,37 +1381,37 @@
       <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="n">
         <v>15.2</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="n">
         <v>8</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="n">
         <v>304</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="n">
         <v>150</v>
       </c>
-      <c r="F24">
+      <c r="F24" t="n">
         <v>3.15</v>
       </c>
-      <c r="G24">
+      <c r="G24" t="n">
         <v>3.435</v>
       </c>
-      <c r="H24">
+      <c r="H24" t="n">
         <v>17.3</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>3</v>
-      </c>
-      <c r="L24">
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>3</v>
+      </c>
+      <c r="L24" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1425,37 +1419,37 @@
       <c r="A25" t="s">
         <v>35</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="n">
         <v>13.3</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="n">
         <v>8</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="n">
         <v>350</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="n">
         <v>245</v>
       </c>
-      <c r="F25">
+      <c r="F25" t="n">
         <v>3.73</v>
       </c>
-      <c r="G25">
+      <c r="G25" t="n">
         <v>3.84</v>
       </c>
-      <c r="H25">
+      <c r="H25" t="n">
         <v>15.41</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>3</v>
-      </c>
-      <c r="L25">
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>3</v>
+      </c>
+      <c r="L25" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1463,37 +1457,37 @@
       <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="n">
         <v>19.2</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="n">
         <v>8</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="n">
         <v>400</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>175</v>
       </c>
-      <c r="F26">
+      <c r="F26" t="n">
         <v>3.08</v>
       </c>
-      <c r="G26">
+      <c r="G26" t="n">
         <v>3.845</v>
       </c>
-      <c r="H26">
+      <c r="H26" t="n">
         <v>17.05</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>3</v>
-      </c>
-      <c r="L26">
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>3</v>
+      </c>
+      <c r="L26" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1501,37 +1495,37 @@
       <c r="A27" t="s">
         <v>37</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="n">
         <v>27.3</v>
       </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27">
+      <c r="C27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" t="n">
         <v>79</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>66</v>
       </c>
-      <c r="F27">
+      <c r="F27" t="n">
         <v>4.08</v>
       </c>
-      <c r="G27">
+      <c r="G27" t="n">
         <v>1.935</v>
       </c>
-      <c r="H27">
+      <c r="H27" t="n">
         <v>18.9</v>
       </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27">
-        <v>4</v>
-      </c>
-      <c r="L27">
+      <c r="I27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" t="n">
+        <v>4</v>
+      </c>
+      <c r="L27" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1539,37 +1533,37 @@
       <c r="A28" t="s">
         <v>38</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="n">
         <v>26</v>
       </c>
-      <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28">
+      <c r="C28" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" t="n">
         <v>120.3</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="n">
         <v>91</v>
       </c>
-      <c r="F28">
+      <c r="F28" t="n">
         <v>4.43</v>
       </c>
-      <c r="G28">
+      <c r="G28" t="n">
         <v>2.14</v>
       </c>
-      <c r="H28">
+      <c r="H28" t="n">
         <v>16.7</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>1</v>
-      </c>
-      <c r="K28">
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" t="n">
         <v>5</v>
       </c>
-      <c r="L28">
+      <c r="L28" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1577,37 +1571,37 @@
       <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="n">
         <v>30.4</v>
       </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <v>95.1</v>
-      </c>
-      <c r="E29">
+      <c r="C29" t="n">
+        <v>4</v>
+      </c>
+      <c r="D29" t="n">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="E29" t="n">
         <v>113</v>
       </c>
-      <c r="F29">
+      <c r="F29" t="n">
         <v>3.77</v>
       </c>
-      <c r="G29">
+      <c r="G29" t="n">
         <v>1.513</v>
       </c>
-      <c r="H29">
+      <c r="H29" t="n">
         <v>16.9</v>
       </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
-      <c r="K29">
+      <c r="I29" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1</v>
+      </c>
+      <c r="K29" t="n">
         <v>5</v>
       </c>
-      <c r="L29">
+      <c r="L29" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1615,37 +1609,37 @@
       <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="n">
         <v>15.8</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="n">
         <v>8</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="n">
         <v>351</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="n">
         <v>264</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="n">
         <v>4.22</v>
       </c>
-      <c r="G30">
+      <c r="G30" t="n">
         <v>3.17</v>
       </c>
-      <c r="H30">
+      <c r="H30" t="n">
         <v>14.5</v>
       </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-      <c r="K30">
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" t="n">
         <v>5</v>
       </c>
-      <c r="L30">
+      <c r="L30" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1653,37 +1647,37 @@
       <c r="A31" t="s">
         <v>41</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="n">
         <v>19.7</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="n">
         <v>6</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="n">
         <v>145</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>175</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="n">
         <v>3.62</v>
       </c>
-      <c r="G31">
+      <c r="G31" t="n">
         <v>2.77</v>
       </c>
-      <c r="H31">
+      <c r="H31" t="n">
         <v>15.5</v>
       </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-      <c r="K31">
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1</v>
+      </c>
+      <c r="K31" t="n">
         <v>5</v>
       </c>
-      <c r="L31">
+      <c r="L31" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1691,37 +1685,37 @@
       <c r="A32" t="s">
         <v>42</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="n">
         <v>15</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="n">
         <v>8</v>
       </c>
-      <c r="D32">
+      <c r="D32" t="n">
         <v>301</v>
       </c>
-      <c r="E32">
+      <c r="E32" t="n">
         <v>335</v>
       </c>
-      <c r="F32">
+      <c r="F32" t="n">
         <v>3.54</v>
       </c>
-      <c r="G32">
+      <c r="G32" t="n">
         <v>3.57</v>
       </c>
-      <c r="H32">
+      <c r="H32" t="n">
         <v>14.6</v>
       </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-      <c r="K32">
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1</v>
+      </c>
+      <c r="K32" t="n">
         <v>5</v>
       </c>
-      <c r="L32">
+      <c r="L32" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1729,41 +1723,41 @@
       <c r="A33" t="s">
         <v>43</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="n">
         <v>21.4</v>
       </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-      <c r="D33">
+      <c r="C33" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" t="n">
         <v>121</v>
       </c>
-      <c r="E33">
+      <c r="E33" t="n">
         <v>109</v>
       </c>
-      <c r="F33">
+      <c r="F33" t="n">
         <v>4.11</v>
       </c>
-      <c r="G33">
+      <c r="G33" t="n">
         <v>2.78</v>
       </c>
-      <c r="H33">
+      <c r="H33" t="n">
         <v>18.6</v>
       </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="K33">
-        <v>4</v>
-      </c>
-      <c r="L33">
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" t="n">
+        <v>4</v>
+      </c>
+      <c r="L33" t="n">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>